<commit_message>
interventions over time in csv output
vectors and vectors0 have to be written out to global variables for this
</commit_message>
<xml_diff>
--- a/Results_Legend_CoMoCOVID-19App.xlsx
+++ b/Results_Legend_CoMoCOVID-19App.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioxfordnexus-my.sharepoint.com/personal/lina3450_ox_ac_uk/Documents/covid19/app related/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="8_{2A2AB986-0296-6548-81A4-6D22AB891699}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EF65F79B-447E-4925-A316-9085E3799C2A}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="8_{2A2AB986-0296-6548-81A4-6D22AB891699}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F8B19C3D-4A09-4B4E-8741-666D76B14466}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8AA8729D-9CF5-B947-9B27-E8E1FEE5F13C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Column name</t>
   </si>
@@ -81,9 +84,6 @@
   </si>
   <si>
     <t xml:space="preserve">Sum of daily reported and unreported incidence. "Predicted Reported + Unreported" line on the graph. </t>
-  </si>
-  <si>
-    <t>*: either for baseline or future scenario</t>
   </si>
   <si>
     <t>*_icu_bed_occupancy</t>
@@ -171,6 +171,69 @@
   </si>
   <si>
     <t>Cumulative non-COVID related deaths in the exposed population (E, I, CL, X, QS, QE, QI, QC, QR, and R compartments) up to time t</t>
+  </si>
+  <si>
+    <t>*_si_vector</t>
+  </si>
+  <si>
+    <t>*_sd_vector</t>
+  </si>
+  <si>
+    <t>*_scr_vector</t>
+  </si>
+  <si>
+    <t>*_hw_vector</t>
+  </si>
+  <si>
+    <t>*_wah_vector</t>
+  </si>
+  <si>
+    <t>*_sc_vector</t>
+  </si>
+  <si>
+    <t>*_tb_vector</t>
+  </si>
+  <si>
+    <t>*_cte_vector</t>
+  </si>
+  <si>
+    <t>*_q_vector</t>
+  </si>
+  <si>
+    <t>*_vc_vector</t>
+  </si>
+  <si>
+    <t>Coverage over time (self-isolation)</t>
+  </si>
+  <si>
+    <t>Coverage over time (social distancing)</t>
+  </si>
+  <si>
+    <t>Coverage over time (screening)</t>
+  </si>
+  <si>
+    <t>Coverage/efficacy over time (handwashing)</t>
+  </si>
+  <si>
+    <t>Coverage over time (working at home)</t>
+  </si>
+  <si>
+    <t>Coverage over time (school closure)</t>
+  </si>
+  <si>
+    <t>Coverage over time (travel ban)</t>
+  </si>
+  <si>
+    <t>Coverage over time (shielding the elderly)</t>
+  </si>
+  <si>
+    <t>Coverage over time (household isolation)</t>
+  </si>
+  <si>
+    <t>Coverage over time (vaccination)</t>
+  </si>
+  <si>
+    <t>*: either for baseline or hypothetical scenario</t>
   </si>
 </sst>
 </file>
@@ -240,8 +303,17 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="COVID19_App_Data(9)"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -541,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81037FD9-033A-114C-BD2B-2883BFFEF60F}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -579,42 +651,42 @@
     </row>
     <row r="4" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
@@ -622,7 +694,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -630,7 +702,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -638,7 +710,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
@@ -646,7 +718,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
@@ -654,7 +726,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
@@ -662,15 +734,15 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
@@ -678,7 +750,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
@@ -686,7 +758,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
@@ -694,7 +766,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
@@ -702,12 +774,92 @@
         <v>3</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>39</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added hospital requirements in csv output
-added hospital requirements in csv output
-change daily_incidence and daily_total_cases to predicted_reported and predicted_reported_and_unreported
</commit_message>
<xml_diff>
--- a/Results_Legend_CoMoCOVID-19App.xlsx
+++ b/Results_Legend_CoMoCOVID-19App.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/CoMo/como/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sai\Documents\GitHub\como\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D8E945-5EA3-C649-8D4A-F3A71FB6C732}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4873EEFB-D30E-445A-BE86-2220E6FB64DC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28000" windowHeight="15840" xr2:uid="{8AA8729D-9CF5-B947-9B27-E8E1FEE5F13C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8AA8729D-9CF5-B947-9B27-E8E1FEE5F13C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Column name</t>
   </si>
@@ -40,12 +40,6 @@
   </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>*_daily_incidence</t>
-  </si>
-  <si>
-    <t>*_daily_total_cases</t>
   </si>
   <si>
     <t>*_cum_mortality</t>
@@ -217,6 +211,30 @@
   </si>
   <si>
     <t>*: either for baseline or hypothetical scenario</t>
+  </si>
+  <si>
+    <t>*_predicted_reported_and_unreported</t>
+  </si>
+  <si>
+    <t>*_predicted_reported</t>
+  </si>
+  <si>
+    <t>*_normal_bed_requirement</t>
+  </si>
+  <si>
+    <t>*_icu_bed_requirement</t>
+  </si>
+  <si>
+    <t>*_icu_ventilator_requirement</t>
+  </si>
+  <si>
+    <t>Patients who require normal inpatient beds</t>
+  </si>
+  <si>
+    <t>Patients who require ICU care, but don't need ventialtor</t>
+  </si>
+  <si>
+    <t>Patients who require ICU care with ventilator</t>
   </si>
 </sst>
 </file>
@@ -583,19 +601,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81037FD9-033A-114C-BD2B-2883BFFEF60F}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="64" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -603,225 +621,249 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="63" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="B16" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="B17" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" s="1" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>45</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>